<commit_message>
export excel and pdf
</commit_message>
<xml_diff>
--- a/Excel Report Barang.xlsx
+++ b/Excel Report Barang.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polmanastraacid-my.sharepoint.com/personal/0320200016_polman_astra_ac_id/Documents/Semester 2/Pemrograman 2/Dosen Industri/QuizMahasiswa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{66C8DE6B-A0D6-4116-8C79-070823AAC182}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A40A743-3192-4AC3-AE5E-762F60EF9E06}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{AAFD6DAE-F662-4BB2-82DF-9F8C6FFC1366}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{B0694F5F-CDAB-4173-A42A-86334EB7C59F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
   <si>
     <t>id_barang</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>PowerBank ACMIC</t>
+  </si>
+  <si>
+    <t>PowerBank Xiaomi</t>
   </si>
 </sst>
 </file>
@@ -441,8 +444,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97585619-B69F-439E-91BA-289BDD811C7E}">
-  <dimension ref="A1:E17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ABD9572-C76C-46D4-AF8E-705B026B155A}">
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -737,6 +740,23 @@
         <v>6</v>
       </c>
     </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18">
+        <v>600000</v>
+      </c>
+      <c r="D18">
+        <v>1000</v>
+      </c>
+      <c r="E18" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>